<commit_message>
Changed a few things
</commit_message>
<xml_diff>
--- a/TA Team Assignment.xlsx
+++ b/TA Team Assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Dela\Documents\Dropbox\_Classes\_3153\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\_Classes\PyCharm Projects\Mixed_File_Types_GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985ACDC5-78DD-4725-A674-8A6E1E5BF24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE36EA51-D008-403B-8448-428686211B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25644" yWindow="528" windowWidth="17124" windowHeight="12732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>TA assigned</t>
   </si>
@@ -419,7 +419,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,15 @@
       <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -592,6 +600,7 @@
     <hyperlink ref="C10" r:id="rId8" display="mailto:soroosh.farsiani@okstate.edu" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="C6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{10EDAB37-4F2C-454A-9802-2ECF5346C5C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>